<commit_message>
new models rum samples saved files
</commit_message>
<xml_diff>
--- a/Dx_1959_Elder_Paper02_Severn.xlsx
+++ b/Dx_1959_Elder_Paper02_Severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Initial Concentration" sheetId="10" r:id="rId3"/>
     <sheet name="Loading" sheetId="3" r:id="rId4"/>
     <sheet name="hidden tab" sheetId="11" r:id="rId5"/>
-    <sheet name="LDC" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="LDC" sheetId="12" r:id="rId6"/>
     <sheet name="چاتا" sheetId="14" state="hidden" r:id="rId7"/>
     <sheet name="ماکیناو" sheetId="15" state="hidden" r:id="rId8"/>
     <sheet name="سورن سفارش نوری" sheetId="13" state="hidden" r:id="rId9"/>
@@ -4680,7 +4680,7 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4928,7 +4928,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="52">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4958,7 +4958,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="52">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -7340,11 +7340,11 @@
       </c>
       <c r="AB2" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>59</v>
+        <v>299</v>
       </c>
       <c r="AC2" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>3.5</v>
+        <v>70</v>
       </c>
       <c r="AD2" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
@@ -7352,7 +7352,7 @@
       </c>
       <c r="AE2" s="75">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF2" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="AJ2" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>485.17318473479997</v>
+        <v>24.258659236739998</v>
       </c>
       <c r="AK2" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="AO2" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="AP2" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -7483,19 +7483,19 @@
       </c>
       <c r="AB3" s="77">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>311</v>
+        <v>1559</v>
       </c>
       <c r="AC3" s="77">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>19.583333333333332</v>
+        <v>391.66666666666669</v>
       </c>
       <c r="AD3" s="77">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>3.5</v>
+        <v>70</v>
       </c>
       <c r="AE3" s="75">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF3" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="AJ3" s="75">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>406.6923060318</v>
+        <v>20.334615301589999</v>
       </c>
       <c r="AK3" s="75">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7533,7 +7533,7 @@
       </c>
       <c r="AO3" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>19</v>
+        <v>391</v>
       </c>
       <c r="AP3" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -7626,19 +7626,19 @@
       </c>
       <c r="AB4" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>815</v>
+        <v>4079</v>
       </c>
       <c r="AC4" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>47.916666666666664</v>
+        <v>958.33333333333337</v>
       </c>
       <c r="AD4" s="84">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>19.583333333333332</v>
+        <v>391.66666666666669</v>
       </c>
       <c r="AE4" s="75">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF4" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7658,7 +7658,7 @@
       </c>
       <c r="AJ4" s="83">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>570.05166895799994</v>
+        <v>28.502583447899994</v>
       </c>
       <c r="AK4" s="83">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7672,7 +7672,7 @@
       <c r="AN4" s="75"/>
       <c r="AO4" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>47</v>
+        <v>958</v>
       </c>
       <c r="AP4" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -7765,19 +7765,19 @@
       </c>
       <c r="AB5" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1776</v>
+        <v>8880</v>
       </c>
       <c r="AC5" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>87.916666666666671</v>
+        <v>1758.3333333333333</v>
       </c>
       <c r="AD5" s="84">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>47.916666666666664</v>
+        <v>958.33333333333337</v>
       </c>
       <c r="AE5" s="75">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7797,7 +7797,7 @@
       </c>
       <c r="AJ5" s="83">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>665.15306118480009</v>
+        <v>33.257653059239999</v>
       </c>
       <c r="AK5" s="83">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7811,7 +7811,7 @@
       <c r="AN5" s="75"/>
       <c r="AO5" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>87</v>
+        <v>1758</v>
       </c>
       <c r="AP5" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -7904,19 +7904,19 @@
       </c>
       <c r="AB6" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>2687</v>
+        <v>13439</v>
       </c>
       <c r="AC6" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>129.58333333333334</v>
+        <v>2591.6666666666665</v>
       </c>
       <c r="AD6" s="84">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>87.916666666666671</v>
+        <v>1758.3333333333333</v>
       </c>
       <c r="AE6" s="75">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7936,7 +7936,7 @@
       </c>
       <c r="AJ6" s="83">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>1105.8344561772001</v>
+        <v>55.291722808860008</v>
       </c>
       <c r="AK6" s="83">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -7950,7 +7950,7 @@
       <c r="AN6" s="75"/>
       <c r="AO6" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>129</v>
+        <v>2591</v>
       </c>
       <c r="AP6" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8043,19 +8043,19 @@
       </c>
       <c r="AB7" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>3623</v>
+        <v>18119</v>
       </c>
       <c r="AC7" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>171.25</v>
+        <v>3425</v>
       </c>
       <c r="AD7" s="84">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>129.58333333333334</v>
+        <v>2591.6666666666665</v>
       </c>
       <c r="AE7" s="75">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF7" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="AJ7" s="83">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>787.92385421159997</v>
+        <v>39.396192710579996</v>
       </c>
       <c r="AK7" s="83">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8089,7 +8089,7 @@
       <c r="AN7" s="75"/>
       <c r="AO7" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>171</v>
+        <v>3425</v>
       </c>
       <c r="AP7" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8182,19 +8182,19 @@
       </c>
       <c r="AB8" s="84">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>4706</v>
+        <v>23532</v>
       </c>
       <c r="AC8" s="84">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>229.58333333333334</v>
+        <v>4591.666666666667</v>
       </c>
       <c r="AD8" s="84">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>171.25</v>
+        <v>3425</v>
       </c>
       <c r="AE8" s="75">
         <f>Delta_T__seconds</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="76">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8214,7 +8214,7 @@
       </c>
       <c r="AJ8" s="83">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>883.62973550519985</v>
+        <v>44.181486775259998</v>
       </c>
       <c r="AK8" s="83">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
@@ -8228,7 +8228,7 @@
       <c r="AN8" s="75"/>
       <c r="AO8" s="99">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>229</v>
+        <v>4591</v>
       </c>
       <c r="AP8" s="99">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
@@ -8432,7 +8432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -8690,7 +8690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:S7"/>
     </sheetView>
   </sheetViews>

</xml_diff>